<commit_message>
added comments excel cnm
</commit_message>
<xml_diff>
--- a/0.SEGUIMIENTO_MAPA.xlsx
+++ b/0.SEGUIMIENTO_MAPA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\poetb\Desktop\Bodega\Map_Whose\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crist\Documents\01.GS\09.Map_revit\Map_Whose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D98C5E-681A-44AB-B97E-770846A95FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E003338C-C01D-4B03-9BD0-F5849E0D8C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1A723B68-A618-4FC2-B49F-C527BEC4ED7D}"/>
+    <workbookView xWindow="-28920" yWindow="-13530" windowWidth="29040" windowHeight="15720" xr2:uid="{1A723B68-A618-4FC2-B49F-C527BEC4ED7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -124,18 +124,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -259,7 +263,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -555,162 +559,174 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C81F392-955F-4CF0-8267-88F20AF3784E}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="14.33203125" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" customWidth="1"/>
-    <col min="10" max="10" width="116.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="I1" s="6">
+        <v>45271</v>
+      </c>
+      <c r="J1" s="6">
+        <v>45272</v>
+      </c>
+      <c r="K1" s="6">
+        <v>45273</v>
+      </c>
+      <c r="L1" s="6">
+        <v>45274</v>
+      </c>
+      <c r="M1" s="6">
+        <v>45275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
       <c r="H3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
       <c r="H4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
       <c r="H5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
       <c r="H6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
       <c r="H7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="4" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:13" ht="86.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -718,9 +734,11 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="A12:G12"/>
+  <mergeCells count="11">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A3:G3"/>

</xml_diff>